<commit_message>
added func for single sheet data entry
</commit_message>
<xml_diff>
--- a/test_data/excel_test.xlsx
+++ b/test_data/excel_test.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:C5"/>
+  <dimension ref="A3:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
@@ -473,6 +473,35 @@
         </is>
       </c>
       <c r="C5" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>Contact</t>
         </is>

</xml_diff>

<commit_message>
minor changes in view
</commit_message>
<xml_diff>
--- a/test_data/excel_test.xlsx
+++ b/test_data/excel_test.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Line Items" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Description" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Extracted Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,9 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b val="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,7 +54,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -419,113 +417,351 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:C7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>Contact</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Contact</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Contact</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Contact</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Contact</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="11" customWidth="1" min="9" max="9"/>
+    <col width="11" customWidth="1" min="10" max="10"/>
+    <col width="14" customWidth="1" min="11" max="11"/>
+    <col width="5" customWidth="1" min="12" max="12"/>
+    <col width="11" customWidth="1" min="13" max="13"/>
+    <col width="18" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="17" max="17"/>
+    <col width="10" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="22" customWidth="1" min="20" max="20"/>
+    <col width="19" customWidth="1" min="21" max="21"/>
+    <col width="35" customWidth="1" min="22" max="22"/>
+    <col width="35" customWidth="1" min="23" max="23"/>
+    <col width="185" customWidth="1" min="24" max="24"/>
+    <col width="16" customWidth="1" min="25" max="25"/>
+    <col width="44" customWidth="1" min="26" max="26"/>
+    <col width="35" customWidth="1" min="27" max="27"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Language</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Document Type</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>Receipt/Invoice No.</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>Reference Numbers</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>Due Date</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>Net Total</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>Total Tax</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>Total Amount</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>Tip</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>Item Code</t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>Item Description</t>
+        </is>
+      </c>
+      <c r="O3" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="Q3" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="R3" s="1" t="inlineStr">
+        <is>
+          <t>Tax Rate</t>
+        </is>
+      </c>
+      <c r="S3" s="1" t="inlineStr">
+        <is>
+          <t>Tax Amount</t>
+        </is>
+      </c>
+      <c r="T3" s="1" t="inlineStr">
+        <is>
+          <t>Supplier Name</t>
+        </is>
+      </c>
+      <c r="U3" s="1" t="inlineStr">
+        <is>
+          <t>Supplier Phone</t>
+        </is>
+      </c>
+      <c r="V3" s="1" t="inlineStr">
+        <is>
+          <t>Supplier Address</t>
+        </is>
+      </c>
+      <c r="W3" s="1" t="inlineStr">
+        <is>
+          <t>Supplier Registration Info</t>
+        </is>
+      </c>
+      <c r="X3" s="1" t="inlineStr">
+        <is>
+          <t>Payment Details</t>
+        </is>
+      </c>
+      <c r="Y3" s="1" t="inlineStr">
+        <is>
+          <t>Customer Name</t>
+        </is>
+      </c>
+      <c r="Z3" s="1" t="inlineStr">
+        <is>
+          <t>Customer Address</t>
+        </is>
+      </c>
+      <c r="AA3" s="1" t="inlineStr">
+        <is>
+          <t>Customer Registration Info</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>02-03-2024</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>08:05 PM</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Expense Receipt</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>80456</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>AP10256, UN5847, AT548R</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>06-04-2024</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>42000</v>
+      </c>
+      <c r="J4" t="n">
+        <v>456.23</v>
+      </c>
+      <c r="K4" t="n">
+        <v>42456.23</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>PRD001</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Widget A</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>10</v>
+      </c>
+      <c r="P4" t="n">
+        <v>25.99</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>259.9</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>25.99</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>John Doe Enterprises</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>+1 (555) 123-4567</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>123 Fake Street, Faketown, FK1234</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Fake Business Registry: ABC123456</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>iban:  GB29 NWBK 6016 1331 9268 19, swift: NWBKGB2L, acc_num: 1234567890, rt_num: 123456789; iban:  GB29 NWBK 6016 1331 9268 19, swift: NWBKGB2L, acc_num: 3658974106, rt_num: 12569843</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Jane Smith Co.</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>456 Imaginary Avenue, Fantasyville, FA5678</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>Fake Business Registry: ABC123456</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>PRD002</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Widget B</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>15.49</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>77.45</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="S5" t="n">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>PRD003</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Widget C</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>20</v>
+      </c>
+      <c r="P6" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>175</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="S6" t="n">
+        <v>8.75</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>